<commit_message>
Alteração do type date nos ficheiros Excel
</commit_message>
<xml_diff>
--- a/SkillEval/public/templates/AddTurmaEAlunos.xlsx
+++ b/SkillEval/public/templates/AddTurmaEAlunos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egcp0\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEB33FD3-CE22-4BEF-B4DE-BE70F96520F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB92FBF3-7BB7-4052-9D02-55C263801553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26475" yWindow="1905" windowWidth="25800" windowHeight="13530" xr2:uid="{9D90FE12-F574-4409-9E91-6B4C243FA39D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9D90FE12-F574-4409-9E91-6B4C243FA39D}"/>
   </bookViews>
   <sheets>
     <sheet name="Turma" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Data de Nascimento (DD/MM/AAAA)</t>
   </si>
   <si>
-    <t>T0000000</t>
-  </si>
-  <si>
     <t>Nome Segundo Terceiro Apelido</t>
   </si>
   <si>
@@ -69,13 +66,16 @@
     <t>Data de Término (DD/MM/AAAA)</t>
   </si>
   <si>
-    <t>99.99</t>
-  </si>
-  <si>
     <t>TPSI</t>
   </si>
   <si>
-    <t>Nome.Apelido.T0000000@atec.pt</t>
+    <t>12.20</t>
+  </si>
+  <si>
+    <t>T0000001</t>
+  </si>
+  <si>
+    <t>Nome.Apelido.T0001000@atec.pt</t>
   </si>
 </sst>
 </file>
@@ -137,17 +137,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -465,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF46FDE-4758-4B11-99E5-88047BD9E66A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,29 +483,29 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>45200</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>45229</v>
       </c>
     </row>
@@ -514,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6655EF3-B27F-452B-A387-9470BB4C8127}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +527,7 @@
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -536,21 +540,21 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="6">
         <v>38139</v>
       </c>
     </row>

</xml_diff>